<commit_message>
Geoparsing data: Cleaning steps 0 to 4
</commit_message>
<xml_diff>
--- a/data/geoparsing/test_geop_results_consistency.xlsx
+++ b/data/geoparsing/test_geop_results_consistency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gael-\Dropbox\Post_doc\Yunne\ORO-map-figures\data\geoparsing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284A4CC6-5350-4CEC-A848-F7E82AB7A934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3C2464-D914-41EE-B965-B3A83B9607E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{847E62F0-F271-4E14-AEA8-DF93AF1BE0E6}"/>
   </bookViews>
@@ -3163,7 +3163,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4773,8 +4773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5EDAF0-BAE3-471B-B88D-3B142F24EE96}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Shame on me aha! I pushed everything at the same time! Cleaning geoparsed data. Updates on figures
</commit_message>
<xml_diff>
--- a/data/geoparsing/test_geop_results_consistency.xlsx
+++ b/data/geoparsing/test_geop_results_consistency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gael-\Dropbox\Post_doc\Yunne\ORO-map-figures\data\geoparsing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3C2464-D914-41EE-B965-B3A83B9607E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51379C0A-C64D-4963-8AFB-F562B5C8800A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{847E62F0-F271-4E14-AEA8-DF93AF1BE0E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5" xr2:uid="{847E62F0-F271-4E14-AEA8-DF93AF1BE0E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Switzerland" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Norway" sheetId="3" r:id="rId3"/>
     <sheet name="United States" sheetId="4" r:id="rId4"/>
     <sheet name="Bottom_countries" sheetId="5" r:id="rId5"/>
+    <sheet name="Test after check" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="583">
   <si>
     <t>analysis_id</t>
   </si>
@@ -2622,6 +2623,576 @@
       </rPr>
       <t>Iraq</t>
     </r>
+  </si>
+  <si>
+    <t>Seagrass metabolism and carbon dynamics in a tropical coastal embayment</t>
+  </si>
+  <si>
+    <t>Sri Lanka, India</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>ture_geoP_location</t>
+  </si>
+  <si>
+    <t>Cell issue because bordering country?</t>
+  </si>
+  <si>
+    <t>ORPC Maine, LLC; Notice of preliminary permit application accepted for filing and soliciting comments, motions to intervene, and competing applications</t>
+  </si>
+  <si>
+    <t>Philippines, Japan, Indonesia</t>
+  </si>
+  <si>
+    <t>An illustrated review on cultivation and life history of agronomically important seaplants</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>United States, Indonesia, Canada</t>
+  </si>
+  <si>
+    <t>Deep biosolids injection: Environmental protection with energy recycling and carbon sequestration</t>
+  </si>
+  <si>
+    <t>Vietnam, Thailand, Indonesia, Guyana</t>
+  </si>
+  <si>
+    <t>Managing erosion of mangrove-mud coasts with permeable dams - lessons learned</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Corrosion protection of offshore wind energy constructions in Germany: Challenges and approaches</t>
+  </si>
+  <si>
+    <t>Partial recovery of microbial function in restored coastal marshes of Oregon, USA</t>
+  </si>
+  <si>
+    <t>Australia, United States</t>
+  </si>
+  <si>
+    <t>Citizen science for monitoring seasonal-scale beach erosion and behaviour with aerial drones</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Border country</t>
+  </si>
+  <si>
+    <t>Recheck after re-run</t>
+  </si>
+  <si>
+    <t>Quantifying gross primary productivity of an Indian mangrove forest using GEO-LEO satellite data</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Sinking failure of scour protection at wind turbine foundation</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Coastal protection against wind-wave induced erosion using soft and porous structures: A case study at Lake Biel, Switzerland</t>
+  </si>
+  <si>
+    <t>Correctable because Country in the title</t>
+  </si>
+  <si>
+    <t>New PU composite is expected to extend German North Sea defenses</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>The value of habitats of conservation importance to climate change mitigation in the UK</t>
+  </si>
+  <si>
+    <t>Aerial surveys of seabirds: The advent of digital methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-occurring Mangroves and Salt Marshes Differ in Microbial Community Composition </t>
+  </si>
+  <si>
+    <t>Indonesia, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The estimation of biomass and carbon stocks in mangrove
+forest ecosystem of Karawang Regency, West Java </t>
+  </si>
+  <si>
+    <t>Carbon stocks in natural and planted mangrove forests of Mahanadi Mangrove Wetland, East Coast of India</t>
+  </si>
+  <si>
+    <t>Seagrass and macrophyte mediated CO2 and CH4 dynamics in shallow coastal waters</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Carbon stocks and accumulation rates in Red Sea seagrass meadows</t>
+  </si>
+  <si>
+    <t>Assessing the influence of ocean acidification to marine amphipods: A comparative study</t>
+  </si>
+  <si>
+    <t>Spain, Brazil</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Carbon Sources Supporting Macro-Invertebrate Communities in Restored Mangrove Forests from Hau Loc, Thanh Hoa, Vietnam</t>
+  </si>
+  <si>
+    <t>United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>Introduced Mangroves Along the Coast of Moloka'i, Hawai'i may Represent Novel Habitats for Megafaunal Communities</t>
+  </si>
+  <si>
+    <t>Brazil, Angola, United States, China</t>
+  </si>
+  <si>
+    <t>Newbuild FPSO corrosion protection - A design and operation planning guideline</t>
+  </si>
+  <si>
+    <t>Response of seagrass 'Blue Carbon' stocks to increased water temperatures</t>
+  </si>
+  <si>
+    <t>Impacts of a geotextile container dune core on marine turtle nesting in Juno Beach, Florida, United States</t>
+  </si>
+  <si>
+    <t>In-ocean experiments of a wave energy conversion device when moored to an anchor and to a drogue</t>
+  </si>
+  <si>
+    <t>Design context for tidal current energy: The Agulhas current stream</t>
+  </si>
+  <si>
+    <t>Mauritus</t>
+  </si>
+  <si>
+    <t>Indian ocean</t>
+  </si>
+  <si>
+    <t>Thaïland</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Spatial-temporal patterns of organic carbon sequestration capacity after long-term coastal wetland reclamation</t>
+  </si>
+  <si>
+    <t>Effect of the conversion of mangroves into shrimp farms on carbon stock in the sediment along the southern Red Sea coast, Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Salt marsh climate change adaptation: Using runnels to adapt to accelerating sea level rise within a drowning New England salt marsh</t>
+  </si>
+  <si>
+    <t>Cuba, United States</t>
+  </si>
+  <si>
+    <t>Sediment accretion and organic carbon burial relative to sea-level rise and storm events in two mangrove forests in Everglades National Park</t>
+  </si>
+  <si>
+    <t>Groundwater Discharge as a Source of Dissolved Carbon and Greenhouse Gases in a Subtropical Estuary</t>
+  </si>
+  <si>
+    <t>United Kingdom, Spain, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eveloping innovative methods to face aquatic invasions in Europe: the Aquainvad-ED project </t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Internation consortium</t>
+  </si>
+  <si>
+    <t>CO2 storage development: status of the large European CCS projects with EEPR funding</t>
+  </si>
+  <si>
+    <t>United Kingdom, Spain</t>
+  </si>
+  <si>
+    <t>Reinforced embankments for the causeway for Pont Briwet Project, Penrhyndeaudreath, North Wales, UK</t>
+  </si>
+  <si>
+    <t>North Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP North Sea Gas Injection Projects: Sustaining Offshore Production </t>
+  </si>
+  <si>
+    <t>Correct with identifying sea names in the title</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Change in fish and benthic communities in Belizean patch reefs in and outside of a marine reserve, across a parrotfish capture ban</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Wind and solar energy utilization for seawater desalination and hydrogen production in the coastal areas of southern Iran</t>
+  </si>
+  <si>
+    <t>Real-time gaseous, PM and ultrafine particle emissions from a modern marine engine operating on biodiesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alliance for Coastal Technologies: Advancing Moored pCO(2) Instruments in Coastal Waters </t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Corrected after check</t>
+  </si>
+  <si>
+    <t>First floating, production storage and offloading vessel in the U.S. Gulf of Mexico</t>
+  </si>
+  <si>
+    <t>Organic chemistry insights for the exceptional soil carbon storage of the seagrass Posidonia australis</t>
+  </si>
+  <si>
+    <t>Benthic Habitat Variations Over Tidal Ridges, North Sea, The Netherlands</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Mobile demersal megafauna at artificial structures in the German Bight - Likely effects of offshore wind farm development</t>
+  </si>
+  <si>
+    <t>Netherlands, Germany, Denmark</t>
+  </si>
+  <si>
+    <t>France, United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>News: Environmental protection: SABIC commissioned LNG-run gas carriers</t>
+  </si>
+  <si>
+    <t>France, UK</t>
+  </si>
+  <si>
+    <t>UK, Myanmar</t>
+  </si>
+  <si>
+    <t>Benthic interactions with renewable energy installations in a temperate ecosystem</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Dublin's saltmarshes contain climate-relevant carbon pools</t>
+  </si>
+  <si>
+    <t>Italy, Greece</t>
+  </si>
+  <si>
+    <t>Effect of explosive shallow hydrothermal vents on delta C-13 and growth performance in the seagrass Posidonia oceanica</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>Greece = Mediterranean sea</t>
+  </si>
+  <si>
+    <t>word == mediterranean sea
+if greece is not the only country, remove greece</t>
+  </si>
+  <si>
+    <t>Organic carbon sequestration and storage in vegetated coastal habitats along the western coast of the Arabian Gulf</t>
+  </si>
+  <si>
+    <t>Arabian Gulf</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Productive instability of coral reef fisheries after climate-driven regime shifts</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Net pay: Economic analysis of a replanted mangrove plantation in Kenya</t>
+  </si>
+  <si>
+    <t>Unites States</t>
+  </si>
+  <si>
+    <t>From tanker-ships to the first FPSO in the US Gom</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Challenges, Lessons Learned, and Successful Implementaions of Multilateral Completion Technology Offshore Abu Dhabi</t>
+  </si>
+  <si>
+    <t>Italy, China</t>
+  </si>
+  <si>
+    <t>Colonization by native species enhances the carbon storage capacity of exotic mangrove monocultures</t>
+  </si>
+  <si>
+    <t>Guangdong is also a brand in Italy</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Natural Variability in Caribbean Coral Physiology and Implications for Coral Bleaching Resilience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caribbean sea </t>
+  </si>
+  <si>
+    <t>Case law</t>
+  </si>
+  <si>
+    <t>How Does Ocean Acidification Affect the Early Life History of Zostera marina? A Series of Experiments Find Parental Carryover Can Benefit Viability or Germination</t>
+  </si>
+  <si>
+    <t>United States, Sweden</t>
+  </si>
+  <si>
+    <t>Consideration regarding the reduction of pollutions emissions by increasing energy efficiency in ship operations</t>
+  </si>
+  <si>
+    <t>High scale, example</t>
+  </si>
+  <si>
+    <t>Impact of coastal defence structures (tetrapods) on a demersal hard-bottom fish community in the southern North Sea</t>
+  </si>
+  <si>
+    <t>Atlantic linked to the USA</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Sustainability in an era of increasing energy demand: Challenges for offshore geotechnics</t>
+  </si>
+  <si>
+    <t>Australasia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Wetlands and global climate change: The role of wetland restoration in a changing world</t>
+  </si>
+  <si>
+    <t>Investigation of fines migration for a high-pressure, high-temperature carbonate gas reservoir offshore Malaysia</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Belowground carbon storage of Micronesian mangrove forests</t>
+  </si>
+  <si>
+    <t>Fuelwood consumption and supply strategies in mangrove forests - Insights from RAMSAR sites in Benin</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Influence of wind direction on intense power fluctuations in large ofshore windfamrs in the North Sea</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>First step in the restoration of a highly degraded coral reef (Singapore) by in situ coral intensive farming</t>
+  </si>
+  <si>
+    <t>Qatar, Italy</t>
+  </si>
+  <si>
+    <t>A New Sustainable and Novel Hybrid Solar Chimney Power Plant Design for Power Generation and Seawater Desalination</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Ireland, USA</t>
+  </si>
+  <si>
+    <t>The Role of the Upper Tidal Estuary in Wetland Blue Carbon Storage and Flux</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Successful offshore application of acid tunneling technology: overcoming the difficulties of high depths, temperatures, and deviations</t>
+  </si>
+  <si>
+    <t>Forecasting range expansion into ecological traps: climate-mediated shifts in sea turtle nesting beaches and human development</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Carbon sequestration and fluxes of restored mangroves in abandoned aquaculture ponds</t>
+  </si>
+  <si>
+    <t>Harnessing Natural Recovery Processes to Improve Restoration Outcomes: An Experimental Assessment of Sponge-Mediated Coral Reef Restoration</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Correctable because the word is a country</t>
+  </si>
+  <si>
+    <t>Enhanced CO2 uptake at a shallow Arctic Ocean seep field overwhelms the positive warming potential of emitted methane</t>
+  </si>
+  <si>
+    <t>Hydrothermal co-solvent processing of marine algae biomass</t>
+  </si>
+  <si>
+    <t>A lab</t>
+  </si>
+  <si>
+    <t>New approach for offshore pile decommissioning with hydraulic presses and floating panels</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Energy from the sea-tidal power</t>
+  </si>
+  <si>
+    <t>Effects of wave energy converters on the surrounding soft-bottom macrofauna (west coast of Sweden)</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Satellite-based wave data and wave energy resource assessment for South China Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaysia </t>
+  </si>
+  <si>
+    <t>Correctable because country in key words</t>
+  </si>
+  <si>
+    <t>Malaysia, Australia</t>
+  </si>
+  <si>
+    <t>Inorganic and Black Carbon Hotspots Constrain Blue Carbon Mitigation Services Across Tropical Seagrass and Temperate Tidal Marshes</t>
+  </si>
+  <si>
+    <t>Mariculture on land-A system for biofuel farming in coastal deserts</t>
+  </si>
+  <si>
+    <t>Mangroves-fisheries linkages - The Malaysian perspective</t>
+  </si>
+  <si>
+    <t>Evaluating, predicting and mapping belowground carbon stores in Kenyan mangroves</t>
+  </si>
+  <si>
+    <t>Assessing the influence of ocean alkalinity enhancement on a coastal phytoplankton community</t>
+  </si>
+  <si>
+    <t>New approach in analysing rock property changes in vuggy carbonates</t>
+  </si>
+  <si>
+    <t>Indonesia, USA, Malaysia</t>
+  </si>
+  <si>
+    <t>Algal Turf Scrubbing: Cleaning Surface Waters with Solar Energy while Producing a Biofuel</t>
+  </si>
+  <si>
+    <t>Drilling and coring systems for shallow water exploration</t>
+  </si>
+  <si>
+    <t>Field methods for amending marine sediment with activated carbon and assessing treatment effectiveness</t>
+  </si>
+  <si>
+    <t>A case study of an offshore seaStation® sea farm</t>
+  </si>
+  <si>
+    <t>USA (Kona)</t>
+  </si>
+  <si>
+    <t>Kona (Hawai) confused with Kona in Japan</t>
+  </si>
+  <si>
+    <t>Ecosystem Development After Mangrove Wetland Creation: Plant-Soil Change Across a 20-Year Chronosequence</t>
+  </si>
+  <si>
+    <t>Permitting of seawater desalination in California: The sand city approach</t>
+  </si>
+  <si>
+    <t>USA, UK, Japan</t>
+  </si>
+  <si>
+    <t>Laboratory simulations and field-study of CO2 seepage in
+aquatic environments</t>
+  </si>
+  <si>
+    <t>Marine reserves help preserve genetic diversity after impacts derived from climate variability: Lessons from the pink abalone in Baja California</t>
+  </si>
+  <si>
+    <t>Mexico, USA</t>
+  </si>
+  <si>
+    <t>Micro-Fragmentation as an Effective and Applied Tool to Restore Remote Reefs in the Eastern Tropical Pacific</t>
+  </si>
+  <si>
+    <t>EDF Paimpol-Brehat tidal current turbine farm: first achievement and preparation for grid connection</t>
+  </si>
+  <si>
+    <t>Climate change challenges and opportunities for seaweed aquaculture in California, the United States</t>
+  </si>
+  <si>
+    <t>Trinidad &amp; Tobago</t>
+  </si>
+  <si>
+    <t>The BP Bombax pipeline project - Design for construction</t>
+  </si>
+  <si>
+    <t>Benthic megafauna and CO2 bubble dynamics observed by underwater photography during a controlled sub-seabed release of CO2</t>
+  </si>
+  <si>
+    <t>Mooring of the veslefrikk b close to the wellhead platform</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Establishment of EEDI Baseline for Inland Ship of Bangladesh</t>
   </si>
 </sst>
 </file>
@@ -2701,7 +3272,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2792,6 +3363,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2805,7 +3394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2844,6 +3433,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4773,8 +5369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5EDAF0-BAE3-471B-B88D-3B142F24EE96}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6963,4 +7559,1904 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8770EFB2-D97C-4D92-84E6-5B5B7BC07436}">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="54.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>258326</v>
+      </c>
+      <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E2" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>413</v>
+      </c>
+      <c r="G2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>351599</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>268987</v>
+      </c>
+      <c r="B4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" t="s">
+        <v>402</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>58270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>61600</v>
+      </c>
+      <c r="B6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" t="s">
+        <v>405</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>323752</v>
+      </c>
+      <c r="B7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E7" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>267943</v>
+      </c>
+      <c r="B8" t="s">
+        <v>409</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7514</v>
+      </c>
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D9" t="s">
+        <v>412</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>260524</v>
+      </c>
+      <c r="B10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10" t="s">
+        <v>396</v>
+      </c>
+      <c r="D10" t="s">
+        <v>396</v>
+      </c>
+      <c r="E10" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>193475</v>
+      </c>
+      <c r="B11" t="s">
+        <v>417</v>
+      </c>
+      <c r="C11" t="s">
+        <v>416</v>
+      </c>
+      <c r="D11" t="s">
+        <v>416</v>
+      </c>
+      <c r="E11" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>362599</v>
+      </c>
+      <c r="B12" t="s">
+        <v>419</v>
+      </c>
+      <c r="C12" t="s">
+        <v>418</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>362541</v>
+      </c>
+      <c r="B13" t="s">
+        <v>421</v>
+      </c>
+      <c r="C13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D13" t="s">
+        <v>407</v>
+      </c>
+      <c r="E13" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>301820</v>
+      </c>
+      <c r="B14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C14" t="s">
+        <v>422</v>
+      </c>
+      <c r="D14" t="s">
+        <v>422</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>351062</v>
+      </c>
+      <c r="B15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15" t="s">
+        <v>422</v>
+      </c>
+      <c r="D15" t="s">
+        <v>422</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>257099</v>
+      </c>
+      <c r="B16" t="s">
+        <v>425</v>
+      </c>
+      <c r="C16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>285159</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="C17" t="s">
+        <v>426</v>
+      </c>
+      <c r="D17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E17" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>36417</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="C18" t="s">
+        <v>396</v>
+      </c>
+      <c r="D18" t="s">
+        <v>396</v>
+      </c>
+      <c r="E18" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>305669</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="C19" t="s">
+        <v>396</v>
+      </c>
+      <c r="D19" t="s">
+        <v>396</v>
+      </c>
+      <c r="E19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>55440</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="C20" t="s">
+        <v>430</v>
+      </c>
+      <c r="D20" t="s">
+        <v>430</v>
+      </c>
+      <c r="E20" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>259651</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="C21" t="s">
+        <v>433</v>
+      </c>
+      <c r="D21" t="s">
+        <v>433</v>
+      </c>
+      <c r="E21" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>61830</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C22" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E22" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>95832</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="C23" t="s">
+        <v>436</v>
+      </c>
+      <c r="D23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>367156</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="C24" t="s">
+        <v>438</v>
+      </c>
+      <c r="D24" t="s">
+        <v>402</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>254968</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" t="s">
+        <v>412</v>
+      </c>
+      <c r="D25" t="s">
+        <v>412</v>
+      </c>
+      <c r="E25" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>115645</v>
+      </c>
+      <c r="B26" t="s">
+        <v>441</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>347168</v>
+      </c>
+      <c r="B27" t="s">
+        <v>442</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>276321</v>
+      </c>
+      <c r="B28" t="s">
+        <v>443</v>
+      </c>
+      <c r="C28" t="s">
+        <v>444</v>
+      </c>
+      <c r="D28" t="s">
+        <v>445</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>253377</v>
+      </c>
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" t="s">
+        <v>446</v>
+      </c>
+      <c r="D29" t="s">
+        <v>446</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>306943</v>
+      </c>
+      <c r="B30" t="s">
+        <v>448</v>
+      </c>
+      <c r="C30" t="s">
+        <v>447</v>
+      </c>
+      <c r="D30" t="s">
+        <v>447</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>305467</v>
+      </c>
+      <c r="B31" t="s">
+        <v>449</v>
+      </c>
+      <c r="C31" t="s">
+        <v>430</v>
+      </c>
+      <c r="D31" t="s">
+        <v>430</v>
+      </c>
+      <c r="E31" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>13138</v>
+      </c>
+      <c r="B32" t="s">
+        <v>450</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>56649</v>
+      </c>
+      <c r="B33" t="s">
+        <v>452</v>
+      </c>
+      <c r="C33" t="s">
+        <v>451</v>
+      </c>
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>262836</v>
+      </c>
+      <c r="B34" t="s">
+        <v>453</v>
+      </c>
+      <c r="C34" t="s">
+        <v>412</v>
+      </c>
+      <c r="D34" t="s">
+        <v>412</v>
+      </c>
+      <c r="E34" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>139750</v>
+      </c>
+      <c r="B35" t="s">
+        <v>455</v>
+      </c>
+      <c r="C35" t="s">
+        <v>454</v>
+      </c>
+      <c r="D35" t="s">
+        <v>456</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>55330</v>
+      </c>
+      <c r="B36" t="s">
+        <v>458</v>
+      </c>
+      <c r="C36" t="s">
+        <v>454</v>
+      </c>
+      <c r="D36" t="s">
+        <v>459</v>
+      </c>
+      <c r="E36" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>323428</v>
+      </c>
+      <c r="B37" t="s">
+        <v>460</v>
+      </c>
+      <c r="C37" t="s">
+        <v>422</v>
+      </c>
+      <c r="D37" t="s">
+        <v>422</v>
+      </c>
+      <c r="E37" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>272443</v>
+      </c>
+      <c r="B38" t="s">
+        <v>462</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" t="s">
+        <v>461</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>51862</v>
+      </c>
+      <c r="B39" t="s">
+        <v>465</v>
+      </c>
+      <c r="C39" t="s">
+        <v>464</v>
+      </c>
+      <c r="D39" t="s">
+        <v>464</v>
+      </c>
+      <c r="E39" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>312388</v>
+      </c>
+      <c r="B40" t="s">
+        <v>467</v>
+      </c>
+      <c r="C40" t="s">
+        <v>466</v>
+      </c>
+      <c r="D40" t="s">
+        <v>466</v>
+      </c>
+      <c r="E40" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>275383</v>
+      </c>
+      <c r="B41" t="s">
+        <v>468</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>181440</v>
+      </c>
+      <c r="B42" t="s">
+        <v>469</v>
+      </c>
+      <c r="C42" t="s">
+        <v>412</v>
+      </c>
+      <c r="D42" t="s">
+        <v>402</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>470</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>347971</v>
+      </c>
+      <c r="B43" t="s">
+        <v>472</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>17531</v>
+      </c>
+      <c r="B44" t="s">
+        <v>473</v>
+      </c>
+      <c r="C44" t="s">
+        <v>412</v>
+      </c>
+      <c r="D44" t="s">
+        <v>412</v>
+      </c>
+      <c r="E44" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>350587</v>
+      </c>
+      <c r="B45" t="s">
+        <v>474</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>475</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>346791</v>
+      </c>
+      <c r="B46" t="s">
+        <v>476</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>477</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>273711</v>
+      </c>
+      <c r="B47" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" t="s">
+        <v>478</v>
+      </c>
+      <c r="D47" t="s">
+        <v>480</v>
+      </c>
+      <c r="E47" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>348090</v>
+      </c>
+      <c r="B48" t="s">
+        <v>482</v>
+      </c>
+      <c r="C48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D48" t="s">
+        <v>483</v>
+      </c>
+      <c r="E48" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>470</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4040</v>
+      </c>
+      <c r="B49" t="s">
+        <v>485</v>
+      </c>
+      <c r="C49" t="s">
+        <v>484</v>
+      </c>
+      <c r="D49" t="s">
+        <v>484</v>
+      </c>
+      <c r="E49" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>3343</v>
+      </c>
+      <c r="B50" t="s">
+        <v>487</v>
+      </c>
+      <c r="C50" t="s">
+        <v>486</v>
+      </c>
+      <c r="D50" t="s">
+        <v>488</v>
+      </c>
+      <c r="E50" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>490</v>
+      </c>
+      <c r="G50" s="30" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>255548</v>
+      </c>
+      <c r="B51" t="s">
+        <v>492</v>
+      </c>
+      <c r="C51" t="s">
+        <v>396</v>
+      </c>
+      <c r="D51" t="s">
+        <v>493</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>102572</v>
+      </c>
+      <c r="B52" t="s">
+        <v>495</v>
+      </c>
+      <c r="C52" t="s">
+        <v>494</v>
+      </c>
+      <c r="D52" t="s">
+        <v>494</v>
+      </c>
+      <c r="E52" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>277863</v>
+      </c>
+      <c r="B53" t="s">
+        <v>497</v>
+      </c>
+      <c r="C53" t="s">
+        <v>496</v>
+      </c>
+      <c r="D53" t="s">
+        <v>496</v>
+      </c>
+      <c r="E53" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>317882</v>
+      </c>
+      <c r="B54" t="s">
+        <v>499</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" t="s">
+        <v>498</v>
+      </c>
+      <c r="E54" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>217263</v>
+      </c>
+      <c r="B55" t="s">
+        <v>501</v>
+      </c>
+      <c r="C55" t="s">
+        <v>500</v>
+      </c>
+      <c r="D55" t="s">
+        <v>500</v>
+      </c>
+      <c r="E55" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>14912</v>
+      </c>
+      <c r="B56" t="s">
+        <v>503</v>
+      </c>
+      <c r="C56" t="s">
+        <v>502</v>
+      </c>
+      <c r="D56" t="s">
+        <v>447</v>
+      </c>
+      <c r="E56" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>49063</v>
+      </c>
+      <c r="B57" t="s">
+        <v>506</v>
+      </c>
+      <c r="C57" t="s">
+        <v>505</v>
+      </c>
+      <c r="D57" t="s">
+        <v>507</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>351036</v>
+      </c>
+      <c r="B58" t="s">
+        <v>508</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>296171</v>
+      </c>
+      <c r="B59" t="s">
+        <v>509</v>
+      </c>
+      <c r="C59" t="s">
+        <v>510</v>
+      </c>
+      <c r="D59" t="s">
+        <v>510</v>
+      </c>
+      <c r="E59" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>301856</v>
+      </c>
+      <c r="B60" t="s">
+        <v>511</v>
+      </c>
+      <c r="C60" t="s">
+        <v>407</v>
+      </c>
+      <c r="D60" t="s">
+        <v>402</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>307894</v>
+      </c>
+      <c r="B61" t="s">
+        <v>513</v>
+      </c>
+      <c r="C61" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" t="s">
+        <v>407</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>489</v>
+      </c>
+      <c r="G61" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>341654</v>
+      </c>
+      <c r="B62" t="s">
+        <v>516</v>
+      </c>
+      <c r="C62" t="s">
+        <v>515</v>
+      </c>
+      <c r="D62" t="s">
+        <v>517</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>279048</v>
+      </c>
+      <c r="B63" t="s">
+        <v>519</v>
+      </c>
+      <c r="C63" t="s">
+        <v>518</v>
+      </c>
+      <c r="D63" t="s">
+        <v>402</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>301821</v>
+      </c>
+      <c r="B64" t="s">
+        <v>520</v>
+      </c>
+      <c r="C64" t="s">
+        <v>515</v>
+      </c>
+      <c r="D64" t="s">
+        <v>515</v>
+      </c>
+      <c r="E64" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>60737</v>
+      </c>
+      <c r="B65" t="s">
+        <v>522</v>
+      </c>
+      <c r="C65" t="s">
+        <v>521</v>
+      </c>
+      <c r="D65" t="s">
+        <v>521</v>
+      </c>
+      <c r="E65" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>207370</v>
+      </c>
+      <c r="B66" t="s">
+        <v>523</v>
+      </c>
+      <c r="C66" t="s">
+        <v>466</v>
+      </c>
+      <c r="D66" t="s">
+        <v>524</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>112</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>363409</v>
+      </c>
+      <c r="B67" t="s">
+        <v>525</v>
+      </c>
+      <c r="C67" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" t="s">
+        <v>461</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>489</v>
+      </c>
+      <c r="G67" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>177244</v>
+      </c>
+      <c r="B68" t="s">
+        <v>527</v>
+      </c>
+      <c r="C68" t="s">
+        <v>526</v>
+      </c>
+      <c r="D68" t="s">
+        <v>526</v>
+      </c>
+      <c r="E68" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>17462</v>
+      </c>
+      <c r="B69" t="s">
+        <v>529</v>
+      </c>
+      <c r="C69" t="s">
+        <v>528</v>
+      </c>
+      <c r="D69" t="s">
+        <v>530</v>
+      </c>
+      <c r="E69" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>47181</v>
+      </c>
+      <c r="B70" t="s">
+        <v>532</v>
+      </c>
+      <c r="C70" t="s">
+        <v>531</v>
+      </c>
+      <c r="D70" t="s">
+        <v>533</v>
+      </c>
+      <c r="E70" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>360769</v>
+      </c>
+      <c r="B71" t="s">
+        <v>535</v>
+      </c>
+      <c r="C71" t="s">
+        <v>534</v>
+      </c>
+      <c r="D71" t="s">
+        <v>534</v>
+      </c>
+      <c r="E71" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>237307</v>
+      </c>
+      <c r="B72" t="s">
+        <v>536</v>
+      </c>
+      <c r="C72" t="s">
+        <v>537</v>
+      </c>
+      <c r="D72" t="s">
+        <v>537</v>
+      </c>
+      <c r="E72" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>59064</v>
+      </c>
+      <c r="B73" t="s">
+        <v>538</v>
+      </c>
+      <c r="C73" t="s">
+        <v>418</v>
+      </c>
+      <c r="D73" t="s">
+        <v>418</v>
+      </c>
+      <c r="E73" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>169761</v>
+      </c>
+      <c r="B74" t="s">
+        <v>539</v>
+      </c>
+      <c r="C74" t="s">
+        <v>534</v>
+      </c>
+      <c r="D74" t="s">
+        <v>540</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>112</v>
+      </c>
+      <c r="G74" s="16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>47892</v>
+      </c>
+      <c r="B75" t="s">
+        <v>542</v>
+      </c>
+      <c r="C75" t="s">
+        <v>71</v>
+      </c>
+      <c r="D75" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>257818</v>
+      </c>
+      <c r="B76" t="s">
+        <v>543</v>
+      </c>
+      <c r="C76" t="s">
+        <v>108</v>
+      </c>
+      <c r="D76" t="s">
+        <v>544</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>470</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>313914</v>
+      </c>
+      <c r="B77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C77" t="s">
+        <v>407</v>
+      </c>
+      <c r="D77" t="s">
+        <v>407</v>
+      </c>
+      <c r="E77" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>383862</v>
+      </c>
+      <c r="B78" t="s">
+        <v>547</v>
+      </c>
+      <c r="C78" t="s">
+        <v>546</v>
+      </c>
+      <c r="D78" t="s">
+        <v>546</v>
+      </c>
+      <c r="E78" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>356798</v>
+      </c>
+      <c r="B79" t="s">
+        <v>548</v>
+      </c>
+      <c r="C79" t="s">
+        <v>549</v>
+      </c>
+      <c r="D79" t="s">
+        <v>549</v>
+      </c>
+      <c r="E79" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>335868</v>
+      </c>
+      <c r="B80" t="s">
+        <v>550</v>
+      </c>
+      <c r="C80" t="s">
+        <v>551</v>
+      </c>
+      <c r="D80" t="s">
+        <v>552</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>112</v>
+      </c>
+      <c r="G80" s="16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>298684</v>
+      </c>
+      <c r="B81" t="s">
+        <v>555</v>
+      </c>
+      <c r="C81" t="s">
+        <v>554</v>
+      </c>
+      <c r="D81" t="s">
+        <v>554</v>
+      </c>
+      <c r="E81" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>381164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>556</v>
+      </c>
+      <c r="C82" t="s">
+        <v>488</v>
+      </c>
+      <c r="D82" t="s">
+        <v>402</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>240191</v>
+      </c>
+      <c r="B83" t="s">
+        <v>557</v>
+      </c>
+      <c r="C83" t="s">
+        <v>552</v>
+      </c>
+      <c r="D83" t="s">
+        <v>552</v>
+      </c>
+      <c r="E83" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>56523</v>
+      </c>
+      <c r="B84" t="s">
+        <v>558</v>
+      </c>
+      <c r="C84" t="s">
+        <v>496</v>
+      </c>
+      <c r="D84" t="s">
+        <v>496</v>
+      </c>
+      <c r="E84" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>267023</v>
+      </c>
+      <c r="B85" t="s">
+        <v>559</v>
+      </c>
+      <c r="C85" t="s">
+        <v>412</v>
+      </c>
+      <c r="D85" t="s">
+        <v>412</v>
+      </c>
+      <c r="E85" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>284750</v>
+      </c>
+      <c r="B86" t="s">
+        <v>560</v>
+      </c>
+      <c r="C86" t="s">
+        <v>561</v>
+      </c>
+      <c r="D86" t="s">
+        <v>515</v>
+      </c>
+      <c r="E86" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>207287</v>
+      </c>
+      <c r="B87" t="s">
+        <v>562</v>
+      </c>
+      <c r="C87" t="s">
+        <v>533</v>
+      </c>
+      <c r="D87" t="s">
+        <v>533</v>
+      </c>
+      <c r="E87" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>381446</v>
+      </c>
+      <c r="B88" t="s">
+        <v>563</v>
+      </c>
+      <c r="C88" t="s">
+        <v>533</v>
+      </c>
+      <c r="D88" t="s">
+        <v>533</v>
+      </c>
+      <c r="E88" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>281048</v>
+      </c>
+      <c r="B89" t="s">
+        <v>564</v>
+      </c>
+      <c r="C89" t="s">
+        <v>533</v>
+      </c>
+      <c r="D89" t="s">
+        <v>533</v>
+      </c>
+      <c r="E89" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>356845</v>
+      </c>
+      <c r="B90" t="s">
+        <v>565</v>
+      </c>
+      <c r="C90" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90" t="s">
+        <v>566</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
+        <v>100</v>
+      </c>
+      <c r="G90" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>174120</v>
+      </c>
+      <c r="B91" t="s">
+        <v>568</v>
+      </c>
+      <c r="C91" t="s">
+        <v>533</v>
+      </c>
+      <c r="D91" t="s">
+        <v>533</v>
+      </c>
+      <c r="E91" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>277896</v>
+      </c>
+      <c r="B92" t="s">
+        <v>569</v>
+      </c>
+      <c r="C92" t="s">
+        <v>533</v>
+      </c>
+      <c r="D92" t="s">
+        <v>533</v>
+      </c>
+      <c r="E92" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>55424</v>
+      </c>
+      <c r="B93" s="29" t="s">
+        <v>571</v>
+      </c>
+      <c r="C93" t="s">
+        <v>570</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>157325</v>
+      </c>
+      <c r="B94" s="29" t="s">
+        <v>572</v>
+      </c>
+      <c r="C94" t="s">
+        <v>573</v>
+      </c>
+      <c r="D94" t="s">
+        <v>573</v>
+      </c>
+      <c r="E94" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>61938</v>
+      </c>
+      <c r="B95" s="29" t="s">
+        <v>574</v>
+      </c>
+      <c r="C95" t="s">
+        <v>533</v>
+      </c>
+      <c r="D95" t="s">
+        <v>537</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>338015</v>
+      </c>
+      <c r="B96" s="29" t="s">
+        <v>575</v>
+      </c>
+      <c r="C96" t="s">
+        <v>546</v>
+      </c>
+      <c r="D96" t="s">
+        <v>546</v>
+      </c>
+      <c r="E96" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>8994</v>
+      </c>
+      <c r="B97" s="29" t="s">
+        <v>576</v>
+      </c>
+      <c r="C97" t="s">
+        <v>533</v>
+      </c>
+      <c r="D97" t="s">
+        <v>533</v>
+      </c>
+      <c r="E97" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>368017</v>
+      </c>
+      <c r="B98" s="29" t="s">
+        <v>578</v>
+      </c>
+      <c r="C98" t="s">
+        <v>577</v>
+      </c>
+      <c r="D98" t="s">
+        <v>577</v>
+      </c>
+      <c r="E98" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>265184</v>
+      </c>
+      <c r="B99" s="29" t="s">
+        <v>579</v>
+      </c>
+      <c r="C99" t="s">
+        <v>422</v>
+      </c>
+      <c r="D99" t="s">
+        <v>422</v>
+      </c>
+      <c r="E99" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>375225</v>
+      </c>
+      <c r="B100" s="29" t="s">
+        <v>580</v>
+      </c>
+      <c r="C100" t="s">
+        <v>71</v>
+      </c>
+      <c r="D100" t="s">
+        <v>71</v>
+      </c>
+      <c r="E100" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>24899</v>
+      </c>
+      <c r="B101" s="29" t="s">
+        <v>582</v>
+      </c>
+      <c r="C101" t="s">
+        <v>581</v>
+      </c>
+      <c r="D101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E101" s="27">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a readme sheet to the geoparsing scoping excel file
</commit_message>
<xml_diff>
--- a/data/geoparsing/test_geop_results_consistency.xlsx
+++ b/data/geoparsing/test_geop_results_consistency.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gael-\Dropbox\Post_doc\Yunne\ORO-map-figures\data\geoparsing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deviv\R-working-folder\ORO-map-figures\data\geoparsing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51379C0A-C64D-4963-8AFB-F562B5C8800A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5" xr2:uid="{847E62F0-F271-4E14-AEA8-DF93AF1BE0E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
-    <sheet name="Switzerland" sheetId="1" r:id="rId1"/>
-    <sheet name="Japan" sheetId="2" r:id="rId2"/>
-    <sheet name="Norway" sheetId="3" r:id="rId3"/>
-    <sheet name="United States" sheetId="4" r:id="rId4"/>
-    <sheet name="Bottom_countries" sheetId="5" r:id="rId5"/>
-    <sheet name="Test after check" sheetId="6" r:id="rId6"/>
+    <sheet name="Read Me" sheetId="7" r:id="rId1"/>
+    <sheet name="Switzerland" sheetId="1" r:id="rId2"/>
+    <sheet name="Japan" sheetId="2" r:id="rId3"/>
+    <sheet name="Norway" sheetId="3" r:id="rId4"/>
+    <sheet name="United States" sheetId="4" r:id="rId5"/>
+    <sheet name="Bottom_countries" sheetId="5" r:id="rId6"/>
+    <sheet name="Test after check" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Gaël Mariani</author>
   </authors>
   <commentList>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{526C0F9C-8ADF-4FD7-AEB9-D0FEBC782DE3}">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{01B168E6-A806-4222-893C-D93B803FFA60}">
+    <comment ref="E30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E39" authorId="0" shapeId="0" xr:uid="{C39AC44F-29AC-4A65-BD3F-11ACFC201A9A}">
+    <comment ref="E39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="587">
   <si>
     <t>analysis_id</t>
   </si>
@@ -3194,11 +3194,23 @@
   <si>
     <t>Establishment of EEDI Baseline for Inland Ship of Bangladesh</t>
   </si>
+  <si>
+    <t>READ ME</t>
+  </si>
+  <si>
+    <t>The first 4 sheets were tests on uncleaned geoparsing data for countries with high numbers of articles attributed to them (Switzerland, Japan, Norway, United States)</t>
+  </si>
+  <si>
+    <t>The 5th sheet performs an analagous check on the bottom 10 countries</t>
+  </si>
+  <si>
+    <t>The last sheet randomly checks100  articles from the entire database (global)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3755,22 +3767,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF6A99C-B3F1-47E1-A0AA-3132E4CC0109}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="36.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.44140625" customWidth="1"/>
-    <col min="6" max="6" width="93.5546875" customWidth="1"/>
+    <col min="2" max="3" width="36.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
+    <col min="5" max="5" width="56.453125" customWidth="1"/>
+    <col min="6" max="6" width="93.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3790,7 +3837,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>47461</v>
       </c>
@@ -3810,7 +3857,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>14787</v>
       </c>
@@ -3830,7 +3877,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>285780</v>
       </c>
@@ -3850,7 +3897,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>355755</v>
       </c>
@@ -3870,7 +3917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>357439</v>
       </c>
@@ -3887,7 +3934,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>79156</v>
       </c>
@@ -3902,7 +3949,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>332827</v>
       </c>
@@ -3919,7 +3966,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>332903</v>
       </c>
@@ -3939,7 +3986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>333623</v>
       </c>
@@ -3959,7 +4006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>333625</v>
       </c>
@@ -3976,7 +4023,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>334867</v>
       </c>
@@ -3996,7 +4043,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>335360</v>
       </c>
@@ -4016,7 +4063,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>336043</v>
       </c>
@@ -4033,7 +4080,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>336044</v>
       </c>
@@ -4050,7 +4097,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>387540</v>
       </c>
@@ -4070,7 +4117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>342317</v>
       </c>
@@ -4090,7 +4137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>14793</v>
       </c>
@@ -4110,7 +4157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>304176</v>
       </c>
@@ -4130,7 +4177,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>26324</v>
       </c>
@@ -4150,7 +4197,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>256051</v>
       </c>
@@ -4176,24 +4223,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A045BD15-7686-4122-8722-A77282296876}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="43.21875" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" customWidth="1"/>
-    <col min="6" max="6" width="78.44140625" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" customWidth="1"/>
+    <col min="6" max="6" width="78.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4213,7 +4260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>382489</v>
       </c>
@@ -4227,7 +4274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>382552</v>
       </c>
@@ -4241,7 +4288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>381785</v>
       </c>
@@ -4261,7 +4308,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>382779</v>
       </c>
@@ -4281,7 +4328,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>382846</v>
       </c>
@@ -4295,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>381454</v>
       </c>
@@ -4315,7 +4362,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>381868</v>
       </c>
@@ -4329,7 +4376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>195253</v>
       </c>
@@ -4349,7 +4396,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>381900</v>
       </c>
@@ -4369,7 +4416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>381962</v>
       </c>
@@ -4383,7 +4430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>323904</v>
       </c>
@@ -4397,7 +4444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>47605</v>
       </c>
@@ -4411,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>274073</v>
       </c>
@@ -4431,7 +4478,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>311214</v>
       </c>
@@ -4451,7 +4498,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>268387</v>
       </c>
@@ -4465,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>195399</v>
       </c>
@@ -4479,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>13292</v>
       </c>
@@ -4499,7 +4546,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6439</v>
       </c>
@@ -4513,7 +4560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>325474</v>
       </c>
@@ -4527,7 +4574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>195060</v>
       </c>
@@ -4549,25 +4596,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801A3FD6-0401-4FA5-B06F-4333C5B9EE2C}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
     <col min="6" max="6" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4587,7 +4634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>212269</v>
       </c>
@@ -4607,7 +4654,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>229654</v>
       </c>
@@ -4627,7 +4674,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>299651</v>
       </c>
@@ -4647,7 +4694,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>348155</v>
       </c>
@@ -4667,7 +4714,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>342097</v>
       </c>
@@ -4687,7 +4734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>258731</v>
       </c>
@@ -4707,7 +4754,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>33956</v>
       </c>
@@ -4727,7 +4774,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>279633</v>
       </c>
@@ -4747,7 +4794,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>351997</v>
       </c>
@@ -4761,7 +4808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>363263</v>
       </c>
@@ -4775,7 +4822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>25251</v>
       </c>
@@ -4795,7 +4842,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>375842</v>
       </c>
@@ -4809,7 +4856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>350395</v>
       </c>
@@ -4829,7 +4876,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>335670</v>
       </c>
@@ -4849,7 +4896,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>318055</v>
       </c>
@@ -4863,7 +4910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>288215</v>
       </c>
@@ -4883,7 +4930,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>335632</v>
       </c>
@@ -4903,7 +4950,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>334720</v>
       </c>
@@ -4917,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>386474</v>
       </c>
@@ -4931,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>149939</v>
       </c>
@@ -4957,24 +5004,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A937D1E-25C3-48A3-BA2E-CDAA047C44D0}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" customWidth="1"/>
-    <col min="6" max="6" width="60.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="36.36328125" customWidth="1"/>
+    <col min="6" max="6" width="60.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4994,7 +5041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>276292</v>
       </c>
@@ -5014,7 +5061,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>378364</v>
       </c>
@@ -5028,7 +5075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>16313</v>
       </c>
@@ -5048,7 +5095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>374419</v>
       </c>
@@ -5068,7 +5115,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>347515</v>
       </c>
@@ -5088,7 +5135,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>195774</v>
       </c>
@@ -5108,7 +5155,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>282821</v>
       </c>
@@ -5125,7 +5172,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>272132</v>
       </c>
@@ -5145,7 +5192,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>253245</v>
       </c>
@@ -5165,7 +5212,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>354773</v>
       </c>
@@ -5185,7 +5232,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>58036</v>
       </c>
@@ -5202,7 +5249,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>365264</v>
       </c>
@@ -5213,7 +5260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>286643</v>
       </c>
@@ -5230,7 +5277,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>356893</v>
       </c>
@@ -5250,7 +5297,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>323932</v>
       </c>
@@ -5270,7 +5317,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>286119</v>
       </c>
@@ -5287,7 +5334,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>55738</v>
       </c>
@@ -5304,7 +5351,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>285266</v>
       </c>
@@ -5324,7 +5371,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>301446</v>
       </c>
@@ -5338,7 +5385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>229112</v>
       </c>
@@ -5355,7 +5402,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="12" t="s">
         <v>131</v>
       </c>
@@ -5365,26 +5412,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5EDAF0-BAE3-471B-B88D-3B142F24EE96}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="98" customWidth="1"/>
-    <col min="3" max="3" width="43.77734375" customWidth="1"/>
-    <col min="4" max="5" width="16.21875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
-    <col min="7" max="7" width="80.44140625" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" customWidth="1"/>
+    <col min="4" max="5" width="16.1796875" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="80.453125" customWidth="1"/>
+    <col min="8" max="8" width="26.6328125" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5413,7 +5460,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3528</v>
       </c>
@@ -5439,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>16553</v>
       </c>
@@ -5465,7 +5512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>18286</v>
       </c>
@@ -5491,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>18996</v>
       </c>
@@ -5514,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>22603</v>
       </c>
@@ -5531,7 +5578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>30597</v>
       </c>
@@ -5554,7 +5601,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>36317</v>
       </c>
@@ -5580,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>43301</v>
       </c>
@@ -5606,7 +5653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>52617</v>
       </c>
@@ -5635,7 +5682,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>57381</v>
       </c>
@@ -5661,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>57536</v>
       </c>
@@ -5678,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>60144</v>
       </c>
@@ -5707,7 +5754,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>60285</v>
       </c>
@@ -5724,7 +5771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>60523</v>
       </c>
@@ -5750,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>99807</v>
       </c>
@@ -5767,7 +5814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>121364</v>
       </c>
@@ -5784,7 +5831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>161159</v>
       </c>
@@ -5807,7 +5854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>191780</v>
       </c>
@@ -5824,7 +5871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>193610</v>
       </c>
@@ -5847,7 +5894,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>197461</v>
       </c>
@@ -5873,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>215502</v>
       </c>
@@ -5896,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>219603</v>
       </c>
@@ -5922,7 +5969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>231360</v>
       </c>
@@ -5939,7 +5986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>253377</v>
       </c>
@@ -5965,7 +6012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>255542</v>
       </c>
@@ -5991,7 +6038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>257061</v>
       </c>
@@ -6017,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>258207</v>
       </c>
@@ -6043,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>260493</v>
       </c>
@@ -6069,7 +6116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>262937</v>
       </c>
@@ -6092,7 +6139,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>263336</v>
       </c>
@@ -6112,7 +6159,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>264509</v>
       </c>
@@ -6135,7 +6182,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>265039</v>
       </c>
@@ -6158,7 +6205,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>267656</v>
       </c>
@@ -6181,7 +6228,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>267964</v>
       </c>
@@ -6204,7 +6251,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>275048</v>
       </c>
@@ -6227,7 +6274,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>282124</v>
       </c>
@@ -6244,7 +6291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>284080</v>
       </c>
@@ -6267,7 +6314,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>284207</v>
       </c>
@@ -6296,7 +6343,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>285032</v>
       </c>
@@ -6319,7 +6366,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>285324</v>
       </c>
@@ -6342,7 +6389,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>291514</v>
       </c>
@@ -6365,7 +6412,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>297372</v>
       </c>
@@ -6388,7 +6435,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>315919</v>
       </c>
@@ -6408,7 +6455,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>319497</v>
       </c>
@@ -6431,7 +6478,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>320615</v>
       </c>
@@ -6454,7 +6501,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>323775</v>
       </c>
@@ -6471,7 +6518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>327175</v>
       </c>
@@ -6488,7 +6535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>331272</v>
       </c>
@@ -6505,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>331656</v>
       </c>
@@ -6525,7 +6572,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>331856</v>
       </c>
@@ -6542,7 +6589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>332675</v>
       </c>
@@ -6562,7 +6609,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>337062</v>
       </c>
@@ -6579,7 +6626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>341885</v>
       </c>
@@ -6602,7 +6649,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>342004</v>
       </c>
@@ -6625,7 +6672,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>344443</v>
       </c>
@@ -6642,7 +6689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>347118</v>
       </c>
@@ -6665,7 +6712,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>349874</v>
       </c>
@@ -6688,7 +6735,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>350996</v>
       </c>
@@ -6705,7 +6752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>351857</v>
       </c>
@@ -6722,7 +6769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>354334</v>
       </c>
@@ -6745,7 +6792,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>355140</v>
       </c>
@@ -6762,7 +6809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>358975</v>
       </c>
@@ -6785,7 +6832,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>359121</v>
       </c>
@@ -6802,7 +6849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>360129</v>
       </c>
@@ -6825,7 +6872,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>364837</v>
       </c>
@@ -6845,7 +6892,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>365146</v>
       </c>
@@ -6862,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>365726</v>
       </c>
@@ -6882,7 +6929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>367947</v>
       </c>
@@ -6899,7 +6946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>369108</v>
       </c>
@@ -6916,7 +6963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>375670</v>
       </c>
@@ -6939,7 +6986,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>375785</v>
       </c>
@@ -6956,7 +7003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>376687</v>
       </c>
@@ -6979,7 +7026,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>380353</v>
       </c>
@@ -6999,7 +7046,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>383492</v>
       </c>
@@ -7019,7 +7066,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>386957</v>
       </c>
@@ -7042,7 +7089,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>388660</v>
       </c>
@@ -7065,7 +7112,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>389071</v>
       </c>
@@ -7088,7 +7135,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>36650</v>
       </c>
@@ -7105,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>41215</v>
       </c>
@@ -7128,7 +7175,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>55421</v>
       </c>
@@ -7145,7 +7192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>201250</v>
       </c>
@@ -7162,7 +7209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>206803</v>
       </c>
@@ -7185,7 +7232,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>227291</v>
       </c>
@@ -7208,7 +7255,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>231428</v>
       </c>
@@ -7228,7 +7275,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>252530</v>
       </c>
@@ -7245,7 +7292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>252776</v>
       </c>
@@ -7265,7 +7312,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>254681</v>
       </c>
@@ -7282,7 +7329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>261036</v>
       </c>
@@ -7305,7 +7352,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>264670</v>
       </c>
@@ -7322,7 +7369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>265156</v>
       </c>
@@ -7345,7 +7392,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>266632</v>
       </c>
@@ -7362,7 +7409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>276251</v>
       </c>
@@ -7385,7 +7432,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>276574</v>
       </c>
@@ -7408,7 +7455,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>314113</v>
       </c>
@@ -7428,7 +7475,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>315732</v>
       </c>
@@ -7451,7 +7498,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>318424</v>
       </c>
@@ -7474,7 +7521,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>321823</v>
       </c>
@@ -7497,7 +7544,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>325352</v>
       </c>
@@ -7517,7 +7564,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>327520</v>
       </c>
@@ -7537,7 +7584,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>336254</v>
       </c>
@@ -7561,25 +7608,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8770EFB2-D97C-4D92-84E6-5B5B7BC07436}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="55.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="55.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" customWidth="1"/>
-    <col min="7" max="7" width="54.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="54.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7602,7 +7649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>258326</v>
       </c>
@@ -7625,7 +7672,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>351599</v>
       </c>
@@ -7642,7 +7689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>268987</v>
       </c>
@@ -7662,7 +7709,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>58270</v>
       </c>
@@ -7682,7 +7729,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>61600</v>
       </c>
@@ -7699,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>323752</v>
       </c>
@@ -7716,7 +7763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>267943</v>
       </c>
@@ -7733,7 +7780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7514</v>
       </c>
@@ -7753,7 +7800,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>260524</v>
       </c>
@@ -7770,7 +7817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>193475</v>
       </c>
@@ -7787,7 +7834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>362599</v>
       </c>
@@ -7810,7 +7857,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>362541</v>
       </c>
@@ -7827,7 +7874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>301820</v>
       </c>
@@ -7844,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>351062</v>
       </c>
@@ -7861,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>257099</v>
       </c>
@@ -7878,7 +7925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>285159</v>
       </c>
@@ -7898,7 +7945,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>36417</v>
       </c>
@@ -7915,7 +7962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>305669</v>
       </c>
@@ -7932,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>55440</v>
       </c>
@@ -7949,7 +7996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>259651</v>
       </c>
@@ -7966,7 +8013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>61830</v>
       </c>
@@ -7983,7 +8030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>95832</v>
       </c>
@@ -8003,7 +8050,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>367156</v>
       </c>
@@ -8023,7 +8070,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>254968</v>
       </c>
@@ -8040,7 +8087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>115645</v>
       </c>
@@ -8057,7 +8104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>347168</v>
       </c>
@@ -8074,7 +8121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>276321</v>
       </c>
@@ -8094,7 +8141,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>253377</v>
       </c>
@@ -8111,7 +8158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>306943</v>
       </c>
@@ -8128,7 +8175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>305467</v>
       </c>
@@ -8145,7 +8192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>13138</v>
       </c>
@@ -8162,7 +8209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>56649</v>
       </c>
@@ -8182,7 +8229,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>262836</v>
       </c>
@@ -8199,7 +8246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>139750</v>
       </c>
@@ -8219,7 +8266,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>55330</v>
       </c>
@@ -8236,7 +8283,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>323428</v>
       </c>
@@ -8253,7 +8300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>272443</v>
       </c>
@@ -8276,7 +8323,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>51862</v>
       </c>
@@ -8293,7 +8340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>312388</v>
       </c>
@@ -8310,7 +8357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>275383</v>
       </c>
@@ -8327,7 +8374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>181440</v>
       </c>
@@ -8350,7 +8397,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>347971</v>
       </c>
@@ -8367,7 +8414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>17531</v>
       </c>
@@ -8384,7 +8431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>350587</v>
       </c>
@@ -8407,7 +8454,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>346791</v>
       </c>
@@ -8427,7 +8474,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>273711</v>
       </c>
@@ -8447,7 +8494,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>348090</v>
       </c>
@@ -8470,7 +8517,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4040</v>
       </c>
@@ -8487,7 +8534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3343</v>
       </c>
@@ -8510,7 +8557,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>255548</v>
       </c>
@@ -8533,7 +8580,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>102572</v>
       </c>
@@ -8550,7 +8597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>277863</v>
       </c>
@@ -8567,7 +8614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>317882</v>
       </c>
@@ -8584,7 +8631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>217263</v>
       </c>
@@ -8601,7 +8648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>14912</v>
       </c>
@@ -8621,7 +8668,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>49063</v>
       </c>
@@ -8641,7 +8688,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>351036</v>
       </c>
@@ -8658,7 +8705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>296171</v>
       </c>
@@ -8675,7 +8722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>301856</v>
       </c>
@@ -8695,7 +8742,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>307894</v>
       </c>
@@ -8718,7 +8765,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>341654</v>
       </c>
@@ -8738,7 +8785,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>279048</v>
       </c>
@@ -8758,7 +8805,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>301821</v>
       </c>
@@ -8775,7 +8822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>60737</v>
       </c>
@@ -8792,7 +8839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>207370</v>
       </c>
@@ -8815,7 +8862,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>363409</v>
       </c>
@@ -8838,7 +8885,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>177244</v>
       </c>
@@ -8855,7 +8902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>17462</v>
       </c>
@@ -8875,7 +8922,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>47181</v>
       </c>
@@ -8895,7 +8942,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>360769</v>
       </c>
@@ -8912,7 +8959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>237307</v>
       </c>
@@ -8929,7 +8976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>59064</v>
       </c>
@@ -8946,7 +8993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>169761</v>
       </c>
@@ -8969,7 +9016,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>47892</v>
       </c>
@@ -8986,7 +9033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>257818</v>
       </c>
@@ -9009,7 +9056,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>313914</v>
       </c>
@@ -9026,7 +9073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>383862</v>
       </c>
@@ -9043,7 +9090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>356798</v>
       </c>
@@ -9060,7 +9107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>335868</v>
       </c>
@@ -9083,7 +9130,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>298684</v>
       </c>
@@ -9100,7 +9147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>381164</v>
       </c>
@@ -9120,7 +9167,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>240191</v>
       </c>
@@ -9137,7 +9184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>56523</v>
       </c>
@@ -9154,7 +9201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>267023</v>
       </c>
@@ -9171,7 +9218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>284750</v>
       </c>
@@ -9191,7 +9238,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>207287</v>
       </c>
@@ -9208,7 +9255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>381446</v>
       </c>
@@ -9225,7 +9272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>281048</v>
       </c>
@@ -9242,7 +9289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>356845</v>
       </c>
@@ -9265,7 +9312,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>174120</v>
       </c>
@@ -9282,7 +9329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>277896</v>
       </c>
@@ -9299,7 +9346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>55424</v>
       </c>
@@ -9316,7 +9363,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>157325</v>
       </c>
@@ -9333,7 +9380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>61938</v>
       </c>
@@ -9353,7 +9400,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>338015</v>
       </c>
@@ -9370,7 +9417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>8994</v>
       </c>
@@ -9387,7 +9434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>368017</v>
       </c>
@@ -9404,7 +9451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>265184</v>
       </c>
@@ -9421,7 +9468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>375225</v>
       </c>
@@ -9438,7 +9485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>24899</v>
       </c>

</xml_diff>